<commit_message>
add rolx debug file
</commit_message>
<xml_diff>
--- a/rolx_fix_client/initiator/rolx_regression_test/report/rex_report.xlsx
+++ b/rolx_fix_client/initiator/rolx_regression_test/report/rex_report.xlsx
@@ -630,7 +630,11 @@
         </is>
       </c>
       <c r="O2" s="4" t="inlineStr"/>
-      <c r="P2" s="4" t="n"/>
+      <c r="P2" s="4" t="inlineStr">
+        <is>
+          <t>failed</t>
+        </is>
+      </c>
       <c r="Q2" s="4" t="inlineStr">
         <is>
           <t>ps:若列表存在failed数据，请查看report.log文件</t>
@@ -707,7 +711,11 @@
         </is>
       </c>
       <c r="O3" s="4" t="inlineStr"/>
-      <c r="P3" s="4" t="n"/>
+      <c r="P3" s="4" t="inlineStr">
+        <is>
+          <t>failed</t>
+        </is>
+      </c>
       <c r="Q3" s="4" t="inlineStr">
         <is>
           <t>Market Price is OK</t>

</xml_diff>